<commit_message>
seperated compiling data code from analysis
</commit_message>
<xml_diff>
--- a/ExcelDataCollection/Complete/DesignOfProcessParametersForProudctionOfXylose.xlsx
+++ b/ExcelDataCollection/Complete/DesignOfProcessParametersForProudctionOfXylose.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\OneDrive\Documents\University\Fourth Year\Thesis\Papers\ExcelDataCollection\Complete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\OneDrive\Documents\University\Fourth Year\Thesis\HemicelluloseThesis\ExcelDataCollection\Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{876B8A6E-9232-4625-9585-79D94D703DAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BBB6A2DD-B55B-4230-A132-7B7F48FAC30A}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{876B8A6E-9232-4625-9585-79D94D703DAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{63EDBD21-44E9-4620-B31A-A9689F7A3616}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" activeTab="2" xr2:uid="{54B929DF-F207-4D70-AA38-DA1517BF04FA}"/>
   </bookViews>
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection activeCell="F6" sqref="F6:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1688,7 +1688,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="F15">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="G15">
         <f t="shared" ref="G15:G33" si="1">250/(D15+1)</f>
@@ -1721,7 +1721,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="F16">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -1754,7 +1754,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="F17">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
@@ -1787,7 +1787,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="F18">
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
@@ -1820,7 +1820,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="F19">
-        <v>5.5</v>
+        <v>0.5</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
@@ -1853,7 +1853,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="F20">
-        <v>6.5</v>
+        <v>0.5</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
@@ -1889,7 +1889,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="F21">
-        <v>7.5</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
@@ -1922,7 +1922,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F22">
-        <v>8.5</v>
+        <v>0.5</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
@@ -1955,7 +1955,7 @@
         <v>1.2156946175120811</v>
       </c>
       <c r="F23">
-        <v>9.5</v>
+        <v>0.5</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
@@ -1988,7 +1988,7 @@
         <v>1.6209261566827746</v>
       </c>
       <c r="F24">
-        <v>10.5</v>
+        <v>0.5</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
@@ -2021,7 +2021,7 @@
         <v>2.0261576958534682</v>
       </c>
       <c r="F25">
-        <v>11.5</v>
+        <v>0.5</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
@@ -2054,7 +2054,7 @@
         <v>2.4313892350241622</v>
       </c>
       <c r="F26">
-        <v>12.5</v>
+        <v>0.5</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
@@ -2081,7 +2081,7 @@
         <v>60</v>
       </c>
       <c r="C27">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D27">
         <v>8</v>
@@ -2090,7 +2090,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F27">
-        <v>13.5</v>
+        <v>0.5</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
@@ -2114,7 +2114,7 @@
         <v>60</v>
       </c>
       <c r="C28">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -2123,7 +2123,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F28">
-        <v>14.5</v>
+        <v>0.5</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
@@ -2147,7 +2147,7 @@
         <v>60</v>
       </c>
       <c r="C29">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D29">
         <v>12</v>
@@ -2156,7 +2156,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F29">
-        <v>15.5</v>
+        <v>0.5</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
@@ -2180,7 +2180,7 @@
         <v>60</v>
       </c>
       <c r="C30">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D30">
         <v>14</v>
@@ -2189,7 +2189,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F30">
-        <v>16.5</v>
+        <v>0.5</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
@@ -2213,7 +2213,7 @@
         <v>60</v>
       </c>
       <c r="C31">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D31">
         <v>16</v>
@@ -2222,7 +2222,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F31">
-        <v>17.5</v>
+        <v>0.5</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
@@ -2246,7 +2246,7 @@
         <v>60</v>
       </c>
       <c r="C32">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D32">
         <v>18</v>
@@ -2255,7 +2255,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F32">
-        <v>18.5</v>
+        <v>0.5</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
@@ -2279,7 +2279,7 @@
         <v>60</v>
       </c>
       <c r="C33">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D33">
         <v>20</v>
@@ -2288,7 +2288,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="F33">
-        <v>19.5</v>
+        <v>0.5</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
@@ -2322,7 +2322,7 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2842,7 +2842,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="E16">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -2874,7 +2874,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="E17">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -2906,7 +2906,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="E18">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="F18">
         <v>3</v>
@@ -2938,7 +2938,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="E19">
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="F19">
         <v>3</v>
@@ -2970,7 +2970,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="E20">
-        <v>5.5</v>
+        <v>0.5</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -3002,7 +3002,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="E21">
-        <v>6.5</v>
+        <v>0.5</v>
       </c>
       <c r="F21">
         <v>3</v>
@@ -3034,7 +3034,7 @@
         <v>0.40523153917069366</v>
       </c>
       <c r="E22">
-        <v>7.5</v>
+        <v>0.5</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -3066,7 +3066,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E23">
-        <v>8.5</v>
+        <v>0.5</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -3098,7 +3098,7 @@
         <v>1.2156946175120811</v>
       </c>
       <c r="E24">
-        <v>9.5</v>
+        <v>0.5</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -3130,7 +3130,7 @@
         <v>1.6209261566827746</v>
       </c>
       <c r="E25">
-        <v>10.5</v>
+        <v>0.5</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -3162,7 +3162,7 @@
         <v>2.0261576958534682</v>
       </c>
       <c r="E26">
-        <v>11.5</v>
+        <v>0.5</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -3194,7 +3194,7 @@
         <v>2.4313892350241622</v>
       </c>
       <c r="E27">
-        <v>12.5</v>
+        <v>0.5</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -3217,7 +3217,7 @@
         <v>60</v>
       </c>
       <c r="B28">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -3226,7 +3226,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E28">
-        <v>13.5</v>
+        <v>0.5</v>
       </c>
       <c r="F28">
         <v>3</v>
@@ -3249,7 +3249,7 @@
         <v>60</v>
       </c>
       <c r="B29">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -3258,7 +3258,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E29">
-        <v>14.5</v>
+        <v>0.5</v>
       </c>
       <c r="F29">
         <v>3</v>
@@ -3281,7 +3281,7 @@
         <v>60</v>
       </c>
       <c r="B30">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C30">
         <v>12</v>
@@ -3290,7 +3290,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E30">
-        <v>15.5</v>
+        <v>0.5</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -3313,7 +3313,7 @@
         <v>60</v>
       </c>
       <c r="B31">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C31">
         <v>14</v>
@@ -3322,7 +3322,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E31">
-        <v>16.5</v>
+        <v>0.5</v>
       </c>
       <c r="F31">
         <v>3</v>
@@ -3345,7 +3345,7 @@
         <v>60</v>
       </c>
       <c r="B32">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -3354,7 +3354,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E32">
-        <v>17.5</v>
+        <v>0.5</v>
       </c>
       <c r="F32">
         <v>3</v>
@@ -3377,7 +3377,7 @@
         <v>60</v>
       </c>
       <c r="B33">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C33">
         <v>18</v>
@@ -3386,7 +3386,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E33">
-        <v>18.5</v>
+        <v>0.5</v>
       </c>
       <c r="F33">
         <v>3</v>
@@ -3409,7 +3409,7 @@
         <v>60</v>
       </c>
       <c r="B34">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C34">
         <v>20</v>
@@ -3418,7 +3418,7 @@
         <v>0.81046307834138731</v>
       </c>
       <c r="E34">
-        <v>19.5</v>
+        <v>0.5</v>
       </c>
       <c r="F34">
         <v>3</v>

</xml_diff>